<commit_message>
Ver 1.11 dashboard consulta
</commit_message>
<xml_diff>
--- a/backend/public/orders/db/orderData-1758305462022.xlsx
+++ b/backend/public/orders/db/orderData-1758305462022.xlsx
@@ -85,7 +85,7 @@
     <t>M</t>
   </si>
   <si>
-    <t>Pendiente</t>
+    <t>Completada</t>
   </si>
   <si>
     <t>1758305462022-2</t>
@@ -623,6 +623,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>